<commit_message>
Remove space from column name
</commit_message>
<xml_diff>
--- a/BaltimoreEmployment/Data/top_employers.xlsx
+++ b/BaltimoreEmployment/Data/top_employers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmaa\Desktop\RShiny\hw2-eyeager\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmaa\Desktop\RShiny\hw2-eyeager1\BaltimoreEmployment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF0AEF1-38E3-4F1A-B675-C07695A895B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D886C4-DE00-4C1D-B2A8-9C4540260B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,17 +51,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Local Employees</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>Industry</t>
     </r>
   </si>
@@ -464,6 +453,9 @@
       </rPr>
       <t>Wegmans Food Markets Inc.</t>
     </r>
+  </si>
+  <si>
+    <t>Employees</t>
   </si>
 </sst>
 </file>
@@ -548,9 +540,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -565,6 +554,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -906,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -926,431 +918,431 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6">
+        <v>25869</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7">
-        <v>25869</v>
-      </c>
-      <c r="D2" s="8" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="6">
+        <v>22142</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7">
-        <v>22142</v>
-      </c>
-      <c r="D3" s="8" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="6">
+        <v>19500</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="7">
-        <v>19500</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="C5" s="6">
+        <v>12385</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="6">
+        <v>9959</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6">
+        <v>8925</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="6">
+        <v>7506</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="6">
+        <v>5284</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="C5" s="7">
-        <v>12385</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="B10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="6">
+        <v>5075</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="C6" s="7">
-        <v>9959</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="B11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="6">
+        <v>5015</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="C7" s="7">
-        <v>8925</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="B12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="6">
+        <v>4485</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
+      <c r="B13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="6">
+        <v>4150</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="C8" s="7">
-        <v>7506</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="B14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="6">
+        <v>4000</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
+      <c r="B15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="6">
+        <v>3900</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="C9" s="7">
-        <v>5284</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="B16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="6">
+        <v>3474</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="7">
-        <v>5075</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="B17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="6">
+        <v>3470</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>16</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="6">
+        <v>3470</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="C11" s="7">
-        <v>5015</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+      <c r="B19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="6">
+        <v>3217</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="6">
+        <v>3168</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="6">
+        <v>3070</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="6">
+        <v>3000</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="6">
+        <v>3000</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="6">
+        <v>2977</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="6">
+        <v>2758</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="6">
+        <v>2600</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="6">
+        <v>2530</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="7">
-        <v>4485</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="7">
-        <v>4150</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="6">
+        <v>2529</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="6">
+        <v>2500</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="6">
+        <v>2301</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="6">
+        <v>2273</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="7">
-        <v>4000</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="7">
-        <v>3900</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
-        <v>15</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="7">
-        <v>3474</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
-        <v>16</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="7">
-        <v>3470</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
-        <v>16</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="7">
-        <v>3470</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
-        <v>18</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="7">
-        <v>3217</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
-        <v>19</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="7">
-        <v>3168</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
-        <v>20</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="7">
-        <v>3070</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
-        <v>21</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="7">
-        <v>3000</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
-        <v>22</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="7">
-        <v>3000</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
-        <v>23</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="7">
-        <v>2977</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
-        <v>24</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="7">
-        <v>2758</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
-        <v>25</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="7">
-        <v>2600</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
-        <v>26</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="7">
-        <v>2530</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
-        <v>27</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="7">
-        <v>2529</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
-        <v>28</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" s="7">
-        <v>2500</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5">
-        <v>29</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="7">
-        <v>2301</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5">
-        <v>30</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="7">
-        <v>2273</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>